<commit_message>
tirei os NAs escritos
</commit_message>
<xml_diff>
--- a/bancos/fifa2018.xlsx
+++ b/bancos/fifa2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvoig\OneDrive\Documentos\curso_R_ABRAJI_28062018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvoig\OneDrive\Documentos\curso_R_ABRAJI_28062018\bancos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13205,8 +13205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M769"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="D220" workbookViewId="0">
+      <selection activeCell="I232" sqref="I232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14234,15 +14234,6 @@
       <c r="I25" t="s">
         <v>837</v>
       </c>
-      <c r="J25" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K25" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L25" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M25" t="s">
         <v>4246</v>
       </c>
@@ -15218,15 +15209,6 @@
       <c r="I49" t="s">
         <v>837</v>
       </c>
-      <c r="J49" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K49" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L49" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M49" t="s">
         <v>4247</v>
       </c>
@@ -16202,15 +16184,6 @@
       <c r="I73" t="s">
         <v>837</v>
       </c>
-      <c r="J73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L73" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M73" t="s">
         <v>4248</v>
       </c>
@@ -17186,15 +17159,6 @@
       <c r="I97" t="s">
         <v>837</v>
       </c>
-      <c r="J97" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K97" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L97" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M97" t="s">
         <v>4249</v>
       </c>
@@ -18170,15 +18134,6 @@
       <c r="I121" t="s">
         <v>837</v>
       </c>
-      <c r="J121" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K121" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L121" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M121" t="s">
         <v>4250</v>
       </c>
@@ -19154,15 +19109,6 @@
       <c r="I145" t="s">
         <v>837</v>
       </c>
-      <c r="J145" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K145" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L145" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M145" t="s">
         <v>4251</v>
       </c>
@@ -20138,15 +20084,6 @@
       <c r="I169" t="s">
         <v>837</v>
       </c>
-      <c r="J169" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K169" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L169" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M169" t="s">
         <v>4252</v>
       </c>
@@ -21122,15 +21059,6 @@
       <c r="I193" t="s">
         <v>837</v>
       </c>
-      <c r="J193" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K193" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L193" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M193" t="s">
         <v>4253</v>
       </c>
@@ -22106,15 +22034,6 @@
       <c r="I217" t="s">
         <v>837</v>
       </c>
-      <c r="J217" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K217" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L217" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M217" t="s">
         <v>4254</v>
       </c>
@@ -23090,15 +23009,6 @@
       <c r="I241" t="s">
         <v>837</v>
       </c>
-      <c r="J241" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K241" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L241" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M241" t="s">
         <v>4255</v>
       </c>
@@ -24074,15 +23984,6 @@
       <c r="I265" t="s">
         <v>837</v>
       </c>
-      <c r="J265" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K265" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L265" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M265" t="s">
         <v>4256</v>
       </c>
@@ -25058,15 +24959,6 @@
       <c r="I289" t="s">
         <v>837</v>
       </c>
-      <c r="J289" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K289" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L289" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M289" t="s">
         <v>4257</v>
       </c>
@@ -26042,15 +25934,6 @@
       <c r="I313" t="s">
         <v>837</v>
       </c>
-      <c r="J313" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K313" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L313" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M313" t="s">
         <v>4258</v>
       </c>
@@ -27026,15 +26909,6 @@
       <c r="I337" t="s">
         <v>837</v>
       </c>
-      <c r="J337" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K337" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L337" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M337" t="s">
         <v>4259</v>
       </c>
@@ -28010,15 +27884,6 @@
       <c r="I361" t="s">
         <v>837</v>
       </c>
-      <c r="J361" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K361" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L361" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M361" t="s">
         <v>4260</v>
       </c>
@@ -28994,15 +28859,6 @@
       <c r="I385" t="s">
         <v>837</v>
       </c>
-      <c r="J385" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K385" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L385" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M385" t="s">
         <v>4261</v>
       </c>
@@ -29978,15 +29834,6 @@
       <c r="I409" t="s">
         <v>837</v>
       </c>
-      <c r="J409" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K409" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L409" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M409" t="s">
         <v>4262</v>
       </c>
@@ -30962,15 +30809,6 @@
       <c r="I433" t="s">
         <v>837</v>
       </c>
-      <c r="J433" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K433" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L433" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M433" t="s">
         <v>4263</v>
       </c>
@@ -31946,15 +31784,6 @@
       <c r="I457" t="s">
         <v>837</v>
       </c>
-      <c r="J457" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K457" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L457" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M457" t="s">
         <v>4264</v>
       </c>
@@ -32930,15 +32759,6 @@
       <c r="I481" t="s">
         <v>837</v>
       </c>
-      <c r="J481" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K481" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L481" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M481" t="s">
         <v>4265</v>
       </c>
@@ -33914,15 +33734,6 @@
       <c r="I505" t="s">
         <v>837</v>
       </c>
-      <c r="J505" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K505" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L505" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M505" t="s">
         <v>4266</v>
       </c>
@@ -34898,15 +34709,6 @@
       <c r="I529" t="s">
         <v>837</v>
       </c>
-      <c r="J529" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K529" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L529" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M529" t="s">
         <v>4267</v>
       </c>
@@ -35882,15 +35684,6 @@
       <c r="I553" t="s">
         <v>837</v>
       </c>
-      <c r="J553" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K553" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L553" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M553" t="s">
         <v>4268</v>
       </c>
@@ -36866,15 +36659,6 @@
       <c r="I577" t="s">
         <v>837</v>
       </c>
-      <c r="J577" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K577" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L577" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M577" t="s">
         <v>4269</v>
       </c>
@@ -37850,15 +37634,6 @@
       <c r="I601" t="s">
         <v>837</v>
       </c>
-      <c r="J601" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K601" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L601" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M601" t="s">
         <v>4270</v>
       </c>
@@ -38834,15 +38609,6 @@
       <c r="I625" t="s">
         <v>837</v>
       </c>
-      <c r="J625" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K625" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L625" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M625" t="s">
         <v>4271</v>
       </c>
@@ -39818,15 +39584,6 @@
       <c r="I649" t="s">
         <v>837</v>
       </c>
-      <c r="J649" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K649" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L649" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M649" t="s">
         <v>4272</v>
       </c>
@@ -40802,15 +40559,6 @@
       <c r="I673" t="s">
         <v>837</v>
       </c>
-      <c r="J673" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K673" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L673" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M673" t="s">
         <v>4273</v>
       </c>
@@ -41786,15 +41534,6 @@
       <c r="I697" t="s">
         <v>837</v>
       </c>
-      <c r="J697" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K697" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L697" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M697" t="s">
         <v>4274</v>
       </c>
@@ -42770,15 +42509,6 @@
       <c r="I721" t="s">
         <v>837</v>
       </c>
-      <c r="J721" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K721" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L721" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M721" t="s">
         <v>4275</v>
       </c>
@@ -43754,15 +43484,6 @@
       <c r="I745" t="s">
         <v>837</v>
       </c>
-      <c r="J745" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K745" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L745" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="M745" t="s">
         <v>4276</v>
       </c>
@@ -44737,15 +44458,6 @@
       </c>
       <c r="I769" t="s">
         <v>837</v>
-      </c>
-      <c r="J769" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K769" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L769" t="e">
-        <v>#N/A</v>
       </c>
       <c r="M769" t="s">
         <v>4277</v>

</xml_diff>